<commit_message>
done with the FTIR and XRD analysis
</commit_message>
<xml_diff>
--- a/Copy of Calibration Curve for Standard methylene dye.xlsx
+++ b/Copy of Calibration Curve for Standard methylene dye.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Emmanuel Project work\Research_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7295933-7494-42B6-827F-099E20BAD0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8999F41-A38D-4DF5-8594-59AEEE05DD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="269" firstSheet="1" activeTab="1" xr2:uid="{3F090771-35F1-4199-9FC6-8E87D1850D2B}"/>
   </bookViews>
@@ -248,23 +248,23 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -798,7 +798,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Adsorption capacity (qe) vs Contact</a:t>
+              <a:t>Adsorption capacity (qt) vs Contact</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -953,20 +953,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1071,20 +1057,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1106,7 +1078,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" b="0"/>
-                  <a:t>Adsorption capacity (qe)</a:t>
+                  <a:t>Adsorption capacity (qt)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1478,20 +1450,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1595,20 +1553,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1991,20 +1935,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2108,20 +2038,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2509,20 +2425,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2631,20 +2533,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3040,20 +2928,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3157,20 +3031,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3565,20 +3425,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3687,20 +3533,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -4094,20 +3926,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -4216,20 +4034,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -6100,20 +5904,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -6217,20 +6007,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -6586,20 +6362,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -6712,20 +6474,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -7074,20 +6822,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -7192,20 +6926,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -7555,20 +7275,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -7672,20 +7378,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -17633,14 +17325,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -17677,7 +17369,7 @@
         <v>0.38932926829268288</v>
       </c>
       <c r="E4">
-        <f>(A4-D4)*(0.01/0.04)</f>
+        <f t="shared" ref="E4:E9" si="0">(A4-D4)*(0.01/0.04)</f>
         <v>1.1526676829268292</v>
       </c>
       <c r="F4">
@@ -17696,15 +17388,15 @@
         <v>0.21617</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D9" si="0">(C5/0.0656)</f>
+        <f t="shared" ref="D5:D9" si="1">(C5/0.0656)</f>
         <v>3.2952743902439021</v>
       </c>
       <c r="E5">
-        <f>(A5-D5)*(0.01/0.04)</f>
+        <f t="shared" si="0"/>
         <v>1.6761814024390245</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5" si="1">((A5-D5)/A5)*100</f>
+        <f t="shared" ref="F5" si="2">((A5-D5)/A5)*100</f>
         <v>67.047256097560975</v>
       </c>
     </row>
@@ -17719,11 +17411,11 @@
         <v>0.40438000000000002</v>
       </c>
       <c r="D6">
+        <f t="shared" si="1"/>
+        <v>6.1643292682926827</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>6.1643292682926827</v>
-      </c>
-      <c r="E6">
-        <f>(A6-D6)*(0.01/0.04)</f>
         <v>2.2089176829268293</v>
       </c>
       <c r="F6">
@@ -17742,11 +17434,11 @@
         <v>0.40143000000000001</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>6.1193597560975608</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>6.1193597560975608</v>
-      </c>
-      <c r="E7">
-        <f>(A7-D7)*(0.01/0.04)</f>
         <v>3.4701600609756098</v>
       </c>
       <c r="F7">
@@ -17765,11 +17457,11 @@
         <v>0.54535999999999996</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>8.3134146341463406</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>8.3134146341463406</v>
-      </c>
-      <c r="E8">
-        <f>(A8-D8)*(0.01/0.04)</f>
         <v>4.1716463414634148</v>
       </c>
       <c r="F8">
@@ -17788,11 +17480,11 @@
         <v>0.16947999999999999</v>
       </c>
       <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2.5835365853658532</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>2.5835365853658532</v>
-      </c>
-      <c r="E9">
-        <f>(A9-D9)*(0.01/0.04)</f>
         <v>11.854115853658536</v>
       </c>
       <c r="F9">
@@ -17811,26 +17503,26 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -17907,7 +17599,7 @@
         <v>0.21695999999999999</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D25" si="2">(C21/0.0636)</f>
+        <f t="shared" ref="D21:D25" si="3">(C21/0.0636)</f>
         <v>3.4113207547169808</v>
       </c>
       <c r="E21">
@@ -17915,19 +17607,19 @@
         <v>1.6471698113207549</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F25" si="3">((A21-D21)/A21)*100</f>
+        <f t="shared" ref="F21:F25" si="4">((A21-D21)/A21)*100</f>
         <v>65.886792452830207</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G25" si="4">D21/E21</f>
+        <f t="shared" ref="G21:G25" si="5">D21/E21</f>
         <v>2.0710194730813285</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:H25" si="5">LOG(E21)</f>
+        <f t="shared" ref="H21:H25" si="6">LOG(E21)</f>
         <v>0.21673837410478072</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:I25" si="6">LOG(D21)</f>
+        <f t="shared" ref="I21:I25" si="7">LOG(D21)</f>
         <v>0.53292255653855547</v>
       </c>
     </row>
@@ -17942,27 +17634,27 @@
         <v>0.40438000000000002</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3581761006289303</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:E25" si="7">(A22-D22)*(0.01/0.04)</f>
+        <f t="shared" ref="E22:E25" si="8">(A22-D22)*(0.01/0.04)</f>
         <v>2.1604559748427672</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>57.612159329140454</v>
       </c>
       <c r="G22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.9429787853426004</v>
       </c>
       <c r="H22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.33454542080801747</v>
       </c>
       <c r="I22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.80333255227838896</v>
       </c>
     </row>
@@ -17977,27 +17669,27 @@
         <v>0.40143000000000001</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3117924528301881</v>
       </c>
       <c r="E23">
+        <f t="shared" si="8"/>
+        <v>3.422051886792453</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>68.441037735849065</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>1.8444467417898616</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="6"/>
+        <v>0.53428659023629377</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="7"/>
-        <v>3.422051886792453</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>68.441037735849065</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="4"/>
-        <v>1.8444467417898616</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="5"/>
-        <v>0.53428659023629377</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="6"/>
         <v>0.80015270977162312</v>
       </c>
     </row>
@@ -18012,27 +17704,27 @@
         <v>0.54535999999999996</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.5748427672955962</v>
       </c>
       <c r="E24">
+        <f t="shared" si="8"/>
+        <v>4.1062893081761009</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>65.700628930817615</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>2.0882217797518758</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
+        <v>0.61344954428401188</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="7"/>
-        <v>4.1062893081761009</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>65.700628930817615</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="4"/>
-        <v>2.0882217797518758</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="5"/>
-        <v>0.61344954428401188</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="6"/>
         <v>0.93322616534198588</v>
       </c>
     </row>
@@ -18047,51 +17739,51 @@
         <v>0.16947999999999999</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.6647798742138362</v>
       </c>
       <c r="E25">
+        <f t="shared" si="8"/>
+        <v>11.833805031446541</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>94.67044025157233</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>0.22518368919655074</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>1.0731244097555586</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="7"/>
-        <v>11.833805031446541</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
-        <v>94.67044025157233</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="4"/>
-        <v>0.22518368919655074</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="5"/>
-        <v>1.0731244097555586</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="6"/>
         <v>0.4256613396805381</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -18151,11 +17843,11 @@
         <v>2.0497382198952878</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E37" si="8">(10-D34)*(0.01/0.04)</f>
+        <f t="shared" ref="E34:E37" si="9">(10-D34)*(0.01/0.04)</f>
         <v>1.9875654450261782</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F37" si="9">((10-D34)/10)*100</f>
+        <f t="shared" ref="F34:F37" si="10">((10-D34)/10)*100</f>
         <v>79.502617801047123</v>
       </c>
     </row>
@@ -18174,11 +17866,11 @@
         <v>6.8227748691099475</v>
       </c>
       <c r="E35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.79430628272251314</v>
       </c>
       <c r="F35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>31.772251308900522</v>
       </c>
     </row>
@@ -18197,11 +17889,11 @@
         <v>6.5238219895287957</v>
       </c>
       <c r="E36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.86904450261780108</v>
       </c>
       <c r="F36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>34.761780104712045</v>
       </c>
     </row>
@@ -18220,11 +17912,11 @@
         <v>5.2390052356020949</v>
       </c>
       <c r="E37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1902486910994763</v>
       </c>
       <c r="F37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>47.609947643979048</v>
       </c>
     </row>
@@ -18348,8 +18040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824E3E7E-C8D3-486C-8AA2-F3D93AAD0389}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18362,14 +18054,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -18411,7 +18103,7 @@
         <v>0.38932926829268288</v>
       </c>
       <c r="E4">
-        <f>(A4-D4)*(0.01/0.04)</f>
+        <f t="shared" ref="E4:E9" si="0">(A4-D4)*(0.01/0.04)</f>
         <v>1.1526676829268292</v>
       </c>
       <c r="F4">
@@ -18430,15 +18122,15 @@
         <v>0.21617</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D9" si="0">(C5/0.0656)</f>
+        <f t="shared" ref="D5:D9" si="1">(C5/0.0656)</f>
         <v>3.2952743902439021</v>
       </c>
       <c r="E5">
-        <f>(A5-D5)*(0.01/0.04)</f>
+        <f t="shared" si="0"/>
         <v>1.6761814024390245</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5" si="1">((A5-D5)/A5)*100</f>
+        <f t="shared" ref="F5" si="2">((A5-D5)/A5)*100</f>
         <v>67.047256097560975</v>
       </c>
     </row>
@@ -18453,11 +18145,11 @@
         <v>0.40438000000000002</v>
       </c>
       <c r="D6">
+        <f t="shared" si="1"/>
+        <v>6.1643292682926827</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>6.1643292682926827</v>
-      </c>
-      <c r="E6">
-        <f>(A6-D6)*(0.01/0.04)</f>
         <v>2.2089176829268293</v>
       </c>
       <c r="F6">
@@ -18476,11 +18168,11 @@
         <v>0.40143000000000001</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>6.1193597560975608</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>6.1193597560975608</v>
-      </c>
-      <c r="E7">
-        <f>(A7-D7)*(0.01/0.04)</f>
         <v>3.4701600609756098</v>
       </c>
       <c r="F7">
@@ -18499,11 +18191,11 @@
         <v>0.54535999999999996</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>8.3134146341463406</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>8.3134146341463406</v>
-      </c>
-      <c r="E8">
-        <f>(A8-D8)*(0.01/0.04)</f>
         <v>4.1716463414634148</v>
       </c>
       <c r="F8">
@@ -18522,11 +18214,11 @@
         <v>0.16947999999999999</v>
       </c>
       <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2.5835365853658532</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>2.5835365853658532</v>
-      </c>
-      <c r="E9">
-        <f>(A9-D9)*(0.01/0.04)</f>
         <v>11.854115853658536</v>
       </c>
       <c r="F9">
@@ -18545,26 +18237,26 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -18620,15 +18312,15 @@
         <v>0.40143000000000001</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D25" si="2">(C21/0.0636)</f>
+        <f t="shared" ref="D21:D25" si="3">(C21/0.0636)</f>
         <v>6.3117924528301881</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E25" si="3">(A21-D21)*(0.01/0.04)</f>
+        <f t="shared" ref="E21:E25" si="4">(A21-D21)*(0.01/0.04)</f>
         <v>0.92205188679245298</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F25" si="4">((A21-D21)/A21)*100</f>
+        <f t="shared" ref="F21:F25" si="5">((A21-D21)/A21)*100</f>
         <v>36.882075471698116</v>
       </c>
     </row>
@@ -18643,15 +18335,15 @@
         <v>0.40438000000000002</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3581761006289303</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.1604559748427672</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57.612159329140454</v>
       </c>
     </row>
@@ -18666,15 +18358,15 @@
         <v>0.21617</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3988993710691822</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.1502751572327048</v>
       </c>
       <c r="F23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83.005503144654085</v>
       </c>
     </row>
@@ -18689,15 +18381,15 @@
         <v>0.16947999999999999</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.6647798742138362</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.5838050314465413</v>
       </c>
       <c r="F24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89.34088050314466</v>
       </c>
     </row>
@@ -18712,39 +18404,39 @@
         <v>2.554E-2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.40157232704402512</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.399606918238995</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99.196855345911956</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -18804,11 +18496,11 @@
         <v>2.0497382198952878</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E37" si="5">(10-D34)*(0.01/0.04)</f>
+        <f t="shared" ref="E34:E37" si="6">(10-D34)*(0.01/0.04)</f>
         <v>1.9875654450261782</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F37" si="6">((10-D34)/10)*100</f>
+        <f t="shared" ref="F34:F37" si="7">((10-D34)/10)*100</f>
         <v>79.502617801047123</v>
       </c>
     </row>
@@ -18827,11 +18519,11 @@
         <v>6.8227748691099475</v>
       </c>
       <c r="E35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.79430628272251314</v>
       </c>
       <c r="F35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>31.772251308900522</v>
       </c>
     </row>
@@ -18850,11 +18542,11 @@
         <v>6.5238219895287957</v>
       </c>
       <c r="E36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.86904450261780108</v>
       </c>
       <c r="F36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>34.761780104712045</v>
       </c>
     </row>
@@ -18873,11 +18565,11 @@
         <v>5.2390052356020949</v>
       </c>
       <c r="E37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1902486910994763</v>
       </c>
       <c r="F37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>47.609947643979048</v>
       </c>
     </row>
@@ -18892,14 +18584,14 @@
       <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="D42" s="3" t="s">
+      <c r="B42" s="9"/>
+      <c r="D42" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="3"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -18935,83 +18627,83 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" ref="A45:A50" si="7">(D21/E21)</f>
+        <f t="shared" ref="A45:A49" si="8">(D21/E21)</f>
         <v>6.8453766466300019</v>
       </c>
       <c r="B45">
-        <f t="shared" ref="B45:B50" si="8">(D21)</f>
+        <f t="shared" ref="B45:B49" si="9">(D21)</f>
         <v>6.3117924528301881</v>
       </c>
       <c r="D45">
-        <f t="shared" ref="D45:D49" si="9">(D34/E34)</f>
+        <f t="shared" ref="D45:D48" si="10">(D34/E34)</f>
         <v>1.0312808692788935</v>
       </c>
       <c r="E45">
-        <f t="shared" ref="E45:E48" si="10">(D34)</f>
+        <f t="shared" ref="E45:E48" si="11">(D34)</f>
         <v>2.0497382198952878</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.9429787853426004</v>
       </c>
       <c r="B46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.3581761006289303</v>
       </c>
       <c r="D46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.5896020433385516</v>
       </c>
       <c r="E46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.8227748691099475</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.81895759734048079</v>
       </c>
       <c r="B47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.3988993710691822</v>
       </c>
       <c r="D47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.5068905791098723</v>
       </c>
       <c r="E47">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.5238219895287957</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.47723368907160751</v>
       </c>
       <c r="B48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.6647798742138362</v>
       </c>
       <c r="D48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.4016055424204117</v>
       </c>
       <c r="E48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.2390052356020949</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.2385891721562483E-2</v>
       </c>
       <c r="B49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.40157232704402512</v>
       </c>
     </row>
@@ -19071,15 +18763,15 @@
         <v>0.95118999999999998</v>
       </c>
       <c r="B56">
-        <f t="shared" ref="B56:B60" si="11">LOG(D21)</f>
+        <f t="shared" ref="B56:B60" si="12">LOG(D21)</f>
         <v>0.80015270977162312</v>
       </c>
       <c r="D56">
-        <f t="shared" ref="D56:D60" si="12">LOG(E34)</f>
+        <f t="shared" ref="D56:D59" si="13">LOG(E34)</f>
         <v>0.29832143767859409</v>
       </c>
       <c r="E56">
-        <f t="shared" ref="E56:E59" si="13">LOG(D34)</f>
+        <f t="shared" ref="E56:E59" si="14">LOG(D34)</f>
         <v>0.31169839914623465</v>
       </c>
     </row>
@@ -19088,15 +18780,15 @@
         <v>1.95119</v>
       </c>
       <c r="B57">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.80333255227838896</v>
       </c>
       <c r="D57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-0.10001200229899405</v>
       </c>
       <c r="E57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.83396104111482539</v>
       </c>
     </row>
@@ -19105,15 +18797,15 @@
         <v>2.95119</v>
       </c>
       <c r="B58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.53133830690836004</v>
       </c>
       <c r="D58">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-6.0957983336751717E-2</v>
       </c>
       <c r="E58">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.81450210227319064</v>
       </c>
     </row>
@@ -19122,15 +18814,15 @@
         <v>3.95119</v>
       </c>
       <c r="B59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.4256613396805381</v>
       </c>
       <c r="D59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7.5637712558993223E-2</v>
       </c>
       <c r="E59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.71924883246053695</v>
       </c>
     </row>
@@ -19139,7 +18831,7 @@
         <v>4.9511900000000004</v>
       </c>
       <c r="B60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.39623622272101744</v>
       </c>
     </row>
@@ -19197,73 +18889,73 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" ref="A66:A69" si="14">E21</f>
+        <f t="shared" ref="A66:A69" si="15">E21</f>
         <v>0.92205188679245298</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B71" si="15">LN(D21)</f>
+        <f t="shared" ref="B66:B70" si="16">LN(D21)</f>
         <v>1.8424197016389305</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D71" si="16">E34</f>
+        <f t="shared" ref="D66:D69" si="17">E34</f>
         <v>1.9875654450261782</v>
       </c>
       <c r="E66">
-        <f t="shared" ref="E66:E70" si="17">LN(D34)</f>
+        <f t="shared" ref="E66:E69" si="18">LN(D34)</f>
         <v>0.71771208738422787</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.1604559748427672</v>
       </c>
       <c r="B67">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.8497415595930782</v>
       </c>
       <c r="D67">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.79430628272251314</v>
       </c>
       <c r="E67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.9202662614087915</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.1502751572327048</v>
       </c>
       <c r="B68">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2234516648238849</v>
       </c>
       <c r="D68">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.86904450261780108</v>
       </c>
       <c r="E68">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.8754603989065604</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.5838050314465413</v>
       </c>
       <c r="B69">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.98012145541228191</v>
       </c>
       <c r="D69">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1902486910994763</v>
       </c>
       <c r="E69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.6561316397770043</v>
       </c>
     </row>
@@ -19273,7 +18965,7 @@
         <v>12.399606918238995</v>
       </c>
       <c r="B70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-0.91236761974168334</v>
       </c>
     </row>
@@ -19282,19 +18974,19 @@
     <sortCondition descending="1" ref="C20:C25"/>
   </sortState>
   <mergeCells count="13">
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A41:F41"/>
     <mergeCell ref="A52:F52"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19312,26 +19004,26 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
chapter 4 almost done
</commit_message>
<xml_diff>
--- a/Copy of Calibration Curve for Standard methylene dye.xlsx
+++ b/Copy of Calibration Curve for Standard methylene dye.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Emmanuel Project work\Research_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8999F41-A38D-4DF5-8594-59AEEE05DD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6893F64D-1BE1-4E24-8F6B-66D538CE48FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="269" firstSheet="1" activeTab="1" xr2:uid="{3F090771-35F1-4199-9FC6-8E87D1850D2B}"/>
   </bookViews>
@@ -145,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,11 +165,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
       </patternFill>
     </fill>
   </fills>
@@ -238,14 +233,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -261,16 +255,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
-    <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1288,19 +1278,8 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Emmanuel Analysis'!$B$43</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ce</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1373,6 +1352,33 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>'Emmanuel Analysis'!$B$44:$B$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.5747851180063517</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3117924528301881</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3581761006289303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3988993710691822</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6647798742138362</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.40157232704402512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>'Emmanuel Analysis'!$A$44:$A$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1394,33 +1400,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.2385891721562483E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Emmanuel Analysis'!$B$44:$B$49</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8.5747851180063517</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.3117924528301881</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.3581761006289303</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.3988993710691822</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.6647798742138362</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.40157232704402512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,19 +2745,8 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Emmanuel Analysis'!$B$54</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Log Ce</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2851,33 +2819,6 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Emmanuel Analysis'!$A$55:$A$60</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>-4.8809999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95118999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.95119</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.95119</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.95119</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.9511900000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>'Emmanuel Analysis'!$B$55:$B$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2899,6 +2840,33 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-0.39623622272101744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Emmanuel Analysis'!$A$55:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.5244639126847867E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33454542080801747</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61807689076183192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74693024571016864</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.093407917747266</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3776,7 +3744,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -3849,6 +3817,33 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>'Emmanuel Analysis'!$B$65:$B$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.1488259336133946</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8424197016389305</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8497415595930782</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2234516648238849</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98012145541228191</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.91236761974168334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>'Emmanuel Analysis'!$A$65:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -3870,33 +3865,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>12.399606918238995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Emmanuel Analysis'!$B$65:$B$70</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.1488259336133946</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.8424197016389305</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8497415595930782</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2234516648238849</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.98012145541228191</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.91236761974168334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16690,14 +16658,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>2721</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>193221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>6803</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>65314</xdr:rowOff>
+      <xdr:rowOff>51707</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18040,8 +18008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824E3E7E-C8D3-486C-8AA2-F3D93AAD0389}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC20" sqref="AC20"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18573,7 +18541,7 @@
         <v>47.609947643979048</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>19</v>
       </c>
@@ -18583,17 +18551,17 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="D42" s="10" t="s">
+      <c r="B42" s="8"/>
+      <c r="D42" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="10"/>
+      <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -18742,8 +18710,9 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>-4.8809999999999999E-2</v>
+      <c r="A55" t="e">
+        <f>LOG(E20)</f>
+        <v>#NUM!</v>
       </c>
       <c r="B55">
         <f>LOG(D20)</f>
@@ -18760,7 +18729,8 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>0.95118999999999998</v>
+        <f>LOG(E21)</f>
+        <v>-3.5244639126847867E-2</v>
       </c>
       <c r="B56">
         <f t="shared" ref="B56:B60" si="12">LOG(D21)</f>
@@ -18777,7 +18747,8 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>1.95119</v>
+        <f t="shared" ref="A57:A60" si="15">LOG(E22)</f>
+        <v>0.33454542080801747</v>
       </c>
       <c r="B57">
         <f t="shared" si="12"/>
@@ -18794,7 +18765,8 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2.95119</v>
+        <f t="shared" si="15"/>
+        <v>0.61807689076183192</v>
       </c>
       <c r="B58">
         <f t="shared" si="12"/>
@@ -18811,7 +18783,8 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>3.95119</v>
+        <f t="shared" si="15"/>
+        <v>0.74693024571016864</v>
       </c>
       <c r="B59">
         <f t="shared" si="12"/>
@@ -18828,7 +18801,8 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>4.9511900000000004</v>
+        <f t="shared" si="15"/>
+        <v>1.093407917747266</v>
       </c>
       <c r="B60">
         <f t="shared" si="12"/>
@@ -18889,73 +18863,73 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" ref="A66:A69" si="15">E21</f>
+        <f t="shared" ref="A66:A69" si="16">E21</f>
         <v>0.92205188679245298</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="16">LN(D21)</f>
+        <f t="shared" ref="B66:B70" si="17">LN(D21)</f>
         <v>1.8424197016389305</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D69" si="17">E34</f>
+        <f t="shared" ref="D66:D69" si="18">E34</f>
         <v>1.9875654450261782</v>
       </c>
       <c r="E66">
-        <f t="shared" ref="E66:E69" si="18">LN(D34)</f>
+        <f t="shared" ref="E66:E69" si="19">LN(D34)</f>
         <v>0.71771208738422787</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.1604559748427672</v>
       </c>
       <c r="B67">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.8497415595930782</v>
       </c>
       <c r="D67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.79430628272251314</v>
       </c>
       <c r="E67">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.9202662614087915</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.1502751572327048</v>
       </c>
       <c r="B68">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.2234516648238849</v>
       </c>
       <c r="D68">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.86904450261780108</v>
       </c>
       <c r="E68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.8754603989065604</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.5838050314465413</v>
       </c>
       <c r="B69">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.98012145541228191</v>
       </c>
       <c r="D69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.1902486910994763</v>
       </c>
       <c r="E69">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.6561316397770043</v>
       </c>
     </row>
@@ -18965,7 +18939,7 @@
         <v>12.399606918238995</v>
       </c>
       <c r="B70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-0.91236761974168334</v>
       </c>
     </row>

</xml_diff>